<commit_message>
aktuelle Koordinaten der neuen Tastatur
</commit_message>
<xml_diff>
--- a/Excel_Tastatur_vermasst.xlsx
+++ b/Excel_Tastatur_vermasst.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f473e8b21b4238c/HF/Softwareentwicklung/Seminarwoche_SE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aschm\OneDrive\Dokumente\GitHub\Seminarwoche\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{FC910521-81CC-44EE-8C07-A43005AF276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36680267-0D8C-4BDE-86EA-3D0796C1EEE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE361E69-29E6-41CE-BF1A-7008B3F20C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D80E5A90-DA00-4670-A347-F110EE1579D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D80E5A90-DA00-4670-A347-F110EE1579D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Leertaste</t>
   </si>
 </sst>
 </file>
@@ -170,22 +173,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -505,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6802DF1-4217-48DB-81F4-AB6B9D3946ED}">
-  <dimension ref="A2:V8"/>
+  <dimension ref="A2:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
@@ -544,305 +541,310 @@
       <c r="U2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
-        <v>-98</v>
+      <c r="C3" s="2">
+        <v>-135</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
-        <v>-79</v>
+      <c r="E3" s="2">
+        <v>-106</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3">
-        <v>-60</v>
+      <c r="G3" s="2">
+        <v>-77</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="3">
-        <v>-41</v>
+      <c r="I3" s="2">
+        <v>-48</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3">
-        <v>-22</v>
+      <c r="K3" s="2">
+        <v>-19</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="3">
-        <v>-3</v>
+      <c r="M3" s="2">
+        <v>10</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="3">
-        <v>16</v>
+      <c r="O3" s="2">
+        <v>39</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="3">
-        <v>35</v>
+      <c r="Q3" s="2">
+        <v>68</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="3">
-        <v>54</v>
+      <c r="S3" s="2">
+        <v>97</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="3">
-        <v>73</v>
-      </c>
-      <c r="V3" s="9">
-        <v>15</v>
+      <c r="U3" s="2">
+        <v>126</v>
+      </c>
+      <c r="V3" s="7">
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="6">
-        <v>197</v>
+      <c r="B4" s="4">
+        <v>213</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
-        <v>197</v>
+      <c r="D4" s="4">
+        <v>213</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="6">
-        <v>197</v>
+      <c r="F4" s="4">
+        <v>213</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="6">
-        <v>197</v>
+      <c r="H4" s="4">
+        <v>213</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="6">
-        <v>197</v>
+      <c r="J4" s="4">
+        <v>213</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="6">
-        <v>197</v>
+      <c r="L4" s="4">
+        <v>213</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="6">
-        <v>197</v>
+      <c r="N4" s="4">
+        <v>213</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="6">
-        <v>197</v>
+      <c r="P4" s="4">
+        <v>213</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="6">
-        <v>197</v>
-      </c>
-      <c r="S4" s="4"/>
-      <c r="T4" s="6">
-        <v>197</v>
+      <c r="R4" s="4">
+        <v>213</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="T4" s="4">
+        <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
-        <v>-94</v>
+      <c r="C5" s="2">
+        <v>-106</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
-        <v>-75</v>
+      <c r="E5" s="2">
+        <v>-77</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="3">
-        <v>-56</v>
+      <c r="G5" s="2">
+        <v>-48</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="3">
-        <v>-37</v>
+      <c r="I5" s="2">
+        <v>-19</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="3">
-        <v>-18</v>
+      <c r="K5" s="2">
+        <v>10</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="3">
-        <v>1</v>
+      <c r="M5" s="2">
+        <v>39</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="3">
-        <v>20</v>
+      <c r="O5" s="2">
+        <v>68</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="3">
-        <v>39</v>
+      <c r="Q5" s="2">
+        <v>97</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="3">
-        <v>58</v>
+      <c r="S5" s="2">
+        <v>126</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="3">
-        <v>77</v>
-      </c>
-      <c r="V5" s="9">
-        <v>13</v>
+      <c r="U5" s="2">
+        <v>155</v>
+      </c>
+      <c r="V5" s="7">
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6">
-        <v>177</v>
+      <c r="B6" s="4">
+        <v>188</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="6">
-        <v>177</v>
+      <c r="D6" s="4">
+        <v>188</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="6">
-        <v>177</v>
+      <c r="F6" s="4">
+        <v>188</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="6">
-        <v>177</v>
+      <c r="H6" s="4">
+        <v>188</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="6">
-        <v>177</v>
+      <c r="J6" s="4">
+        <v>188</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="6">
-        <v>177</v>
+      <c r="L6" s="4">
+        <v>188</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="6">
-        <v>177</v>
+      <c r="N6" s="4">
+        <v>188</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="6">
-        <v>177</v>
+      <c r="P6" s="4">
+        <v>188</v>
       </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="6">
-        <v>177</v>
+      <c r="R6" s="4">
+        <v>188</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="6">
-        <v>177</v>
+      <c r="T6" s="4">
+        <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3">
-        <v>-85</v>
+      <c r="C7" s="2">
+        <v>-106</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3">
-        <v>-66</v>
+      <c r="E7" s="2">
+        <v>-77</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="3">
-        <v>-47</v>
+      <c r="G7" s="2">
+        <v>-48</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="3">
-        <v>-28</v>
+      <c r="I7" s="2">
+        <v>-19</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="3">
-        <v>-9</v>
+      <c r="K7" s="2">
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="3">
-        <v>10</v>
+      <c r="M7" s="2">
+        <v>39</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="3">
-        <v>29</v>
-      </c>
-      <c r="V7" s="9">
-        <v>11</v>
+      <c r="O7" s="2">
+        <v>68</v>
+      </c>
+      <c r="V7" s="7">
+        <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6">
-        <v>157</v>
-      </c>
-      <c r="D8" s="6">
-        <v>157</v>
+      <c r="B8" s="4">
+        <v>163</v>
+      </c>
+      <c r="D8" s="4">
+        <v>163</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="6">
-        <v>157</v>
+      <c r="F8" s="4">
+        <v>163</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="6">
-        <v>157</v>
+      <c r="H8" s="4">
+        <v>163</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="6">
-        <v>157</v>
+      <c r="J8" s="4">
+        <v>163</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="6">
-        <v>157</v>
+      <c r="L8" s="4">
+        <v>163</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="6">
-        <v>157</v>
+      <c r="N8" s="4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -863,15 +865,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010002B2E55CEBBCAB4A8DA6769F06AE0CFF" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="714eb74623d0f643779335d08082c52e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64156f10-9f12-4447-a2c0-ceef305ce254" xmlns:ns3="e1205da7-1578-4715-b515-c64bbb3bce98" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="92831205aad5f9f6ba351692aadbbf5e" ns2:_="" ns3:_="">
     <xsd:import namespace="64156f10-9f12-4447-a2c0-ceef305ce254"/>
@@ -1060,6 +1053,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED5EFE08-EAFC-4C87-9F09-0C27E6D473C3}">
   <ds:schemaRefs>
@@ -1072,14 +1074,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{410419B3-7295-4BE2-A38F-8E480EA267E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A56DD310-0C11-4BE1-9FBC-F5BF4EEF37AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1096,4 +1090,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{410419B3-7295-4BE2-A38F-8E480EA267E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>